<commit_message>
Modification of S6 Table
</commit_message>
<xml_diff>
--- a/supplementary/S6_Table.xlsx
+++ b/supplementary/S6_Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maylis\Dropbox\Systematic review\Supplementary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maylis\Documents\cfss\RabiesScopingReview\supplementary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3378AECF-CCB6-465E-AD2B-920195E0ACF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCCD759-2DF0-4CAC-90BC-DF2B1C1C42D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="372" windowWidth="23256" windowHeight="12696" xr2:uid="{153CD5C9-7E4D-403C-8516-3F0E209DA807}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="103">
   <si>
     <t>Location</t>
   </si>
@@ -1123,6 +1123,15 @@
   </si>
   <si>
     <t>S6 Table. Detailed list of the estimated parameters in mathematical models.</t>
+  </si>
+  <si>
+    <t>Study category</t>
+  </si>
+  <si>
+    <t>Mathematical modelling</t>
+  </si>
+  <si>
+    <t>Interdisciplinary</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1261,12 +1270,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -1415,6 +1425,25 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1506,10 +1535,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{564B6CAB-9B3E-4101-99F2-B1AA3A321FF7}" name="Table5" displayName="Table5" ref="A3:G29" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A3:G29" xr:uid="{60E74816-D9BA-49C1-BDE6-4503AABE2C70}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A8E8D57E-3ACD-42C4-84EB-332380DEE413}" name="Location" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{564B6CAB-9B3E-4101-99F2-B1AA3A321FF7}" name="Table5" displayName="Table5" ref="A3:H29" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A3:H29" xr:uid="{60E74816-D9BA-49C1-BDE6-4503AABE2C70}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{A8E8D57E-3ACD-42C4-84EB-332380DEE413}" name="Study category" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{2A864CC3-E58C-4C19-88DB-988AEFF043F2}" name="Location" dataDxfId="6"/>
     <tableColumn id="7" xr3:uid="{E1555418-5ADD-46DB-B294-0B5B1692C54D}" name="Reproduction ratio" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{A881A2AE-B262-458D-AE80-784B00592727}" name="Transmission rates_x000a_(95% CI)" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{C4A20350-4F28-42EB-A363-C218C53F2CF8}" name="Rabies-related parameters_x000a_(95% CI)" dataDxfId="3"/>
@@ -1818,148 +1848,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C713342-D9CF-4C1C-9AC6-DEFAF1E0B650}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.109375" customWidth="1"/>
-    <col min="2" max="3" width="61.6640625" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" customWidth="1"/>
-    <col min="6" max="6" width="34.88671875" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="58.109375" customWidth="1"/>
+    <col min="3" max="4" width="61.6640625" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="34.88671875" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="B1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1969,43 +2033,49 @@
       <c r="F8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="70.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:8" ht="70.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="E9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D10" s="7" t="s">
         <v>9</v>
       </c>
@@ -2015,20 +2085,23 @@
       <c r="F10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
@@ -2038,20 +2111,23 @@
       <c r="F11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D12" s="7" t="s">
         <v>9</v>
       </c>
@@ -2061,66 +2137,75 @@
       <c r="F12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="E13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="E14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:8" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D15" s="7" t="s">
         <v>9</v>
       </c>
@@ -2130,20 +2215,23 @@
       <c r="F15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D16" s="7" t="s">
         <v>9</v>
       </c>
@@ -2153,20 +2241,23 @@
       <c r="F16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D17" s="7" t="s">
         <v>9</v>
       </c>
@@ -2176,20 +2267,23 @@
       <c r="F17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D18" s="7" t="s">
         <v>9</v>
       </c>
@@ -2199,158 +2293,179 @@
       <c r="F18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="42" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="F19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="70.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:8" ht="70.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="E20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="97.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:8" ht="97.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="F21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="70.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:8" ht="70.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="E22" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="H22" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="160.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:8" ht="160.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="C23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="160.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:8" ht="160.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="C24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="F24" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="G24" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D25" s="7" t="s">
         <v>9</v>
       </c>
@@ -2360,20 +2475,23 @@
       <c r="F25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D26" s="7" t="s">
         <v>9</v>
       </c>
@@ -2383,20 +2501,23 @@
       <c r="F26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D27" s="7" t="s">
         <v>9</v>
       </c>
@@ -2406,20 +2527,23 @@
       <c r="F27" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D28" s="7" t="s">
         <v>9</v>
       </c>
@@ -2429,20 +2553,23 @@
       <c r="F28" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D29" s="7" t="s">
         <v>9</v>
       </c>
@@ -2450,58 +2577,64 @@
         <v>9</v>
       </c>
       <c r="F29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="H29" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+    <row r="31" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
         <v>96</v>
       </c>
       <c r="B31" s="10"/>
-    </row>
-    <row r="32" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>97</v>
       </c>
       <c r="B32" s="11"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="11"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>98</v>
       </c>
       <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G10" r:id="rId1" xr:uid="{262F79F8-AB95-4BD1-8D75-4FAE7544EA04}"/>
-    <hyperlink ref="G15" r:id="rId2" xr:uid="{C6358F64-F5E9-4DBF-ADA0-F5EBCE402570}"/>
-    <hyperlink ref="G11" r:id="rId3" xr:uid="{D17D754C-41A0-4798-B615-06E0FB7C2E64}"/>
-    <hyperlink ref="G24" r:id="rId4" xr:uid="{5033774E-72EF-42D2-B3C0-4F727D318833}"/>
-    <hyperlink ref="G29" r:id="rId5" xr:uid="{B10EE176-2F48-4FC1-90A1-E76C2D82B4D2}"/>
-    <hyperlink ref="G12" r:id="rId6" xr:uid="{E6D24467-5C7A-44AF-B1D5-E36396A9A810}"/>
-    <hyperlink ref="G18" r:id="rId7" xr:uid="{EF37296B-2C4F-443E-8A62-5EBC2C7C912D}"/>
-    <hyperlink ref="G25" r:id="rId8" xr:uid="{D5CCAD84-AA32-46C6-8982-ED0BE724ED24}"/>
-    <hyperlink ref="G13" r:id="rId9" xr:uid="{1C4D161B-5B9A-48D8-8915-791C7D0D57F6}"/>
-    <hyperlink ref="G28" r:id="rId10" xr:uid="{A3E534BB-E017-4FD6-8571-6B29D0EC1106}"/>
-    <hyperlink ref="G9" r:id="rId11" xr:uid="{3A11E16B-FDBC-4C11-A8B9-5D70D3AF6CE1}"/>
-    <hyperlink ref="G8" r:id="rId12" xr:uid="{D967CC38-902E-4CFB-B295-BD12ED14CF46}"/>
-    <hyperlink ref="G21" r:id="rId13" xr:uid="{AA4253AA-A5F9-4D33-9C0C-D0D54386A28A}"/>
-    <hyperlink ref="G19" r:id="rId14" xr:uid="{E0CE1F9E-1805-40CE-ABC5-B9DD1FCAF543}"/>
-    <hyperlink ref="G22" r:id="rId15" xr:uid="{C8DA5180-F0CB-402F-8319-619DD97F760F}"/>
-    <hyperlink ref="G20" r:id="rId16" xr:uid="{FB4130F6-3C25-45EC-AA00-61634945DC3F}"/>
-    <hyperlink ref="G4" r:id="rId17" xr:uid="{EEA2A48A-87FD-4482-91B9-1FF201ECBDFE}"/>
-    <hyperlink ref="G5" r:id="rId18" xr:uid="{E1474B6E-8B4D-40B5-AB1E-FA6B4DD997D8}"/>
-    <hyperlink ref="G6" r:id="rId19" xr:uid="{BF7882F2-1EF5-456D-AC58-8DC01C06893D}"/>
-    <hyperlink ref="G7" r:id="rId20" xr:uid="{478BB94C-435A-440D-9965-610D80EE4528}"/>
-    <hyperlink ref="G14" r:id="rId21" xr:uid="{9F355800-7535-4B88-B262-C64C59E477C1}"/>
-    <hyperlink ref="G16" r:id="rId22" xr:uid="{DC75FD14-51FF-4299-9C9A-7D20A6F25D29}"/>
-    <hyperlink ref="G17" r:id="rId23" xr:uid="{5231848B-A283-4A46-840C-2C91C3616795}"/>
-    <hyperlink ref="G23" r:id="rId24" xr:uid="{017F9B11-4368-4CA1-A199-7BA86CC8FE01}"/>
-    <hyperlink ref="G26" r:id="rId25" xr:uid="{B5B7B496-3341-43BE-85CE-3C243D1EB096}"/>
-    <hyperlink ref="G27" r:id="rId26" xr:uid="{1C7CDA99-49DC-41E9-AA06-FEE25BA3567E}"/>
+    <hyperlink ref="H10" r:id="rId1" xr:uid="{262F79F8-AB95-4BD1-8D75-4FAE7544EA04}"/>
+    <hyperlink ref="H15" r:id="rId2" xr:uid="{C6358F64-F5E9-4DBF-ADA0-F5EBCE402570}"/>
+    <hyperlink ref="H11" r:id="rId3" xr:uid="{D17D754C-41A0-4798-B615-06E0FB7C2E64}"/>
+    <hyperlink ref="H24" r:id="rId4" xr:uid="{5033774E-72EF-42D2-B3C0-4F727D318833}"/>
+    <hyperlink ref="H29" r:id="rId5" xr:uid="{B10EE176-2F48-4FC1-90A1-E76C2D82B4D2}"/>
+    <hyperlink ref="H12" r:id="rId6" xr:uid="{E6D24467-5C7A-44AF-B1D5-E36396A9A810}"/>
+    <hyperlink ref="H18" r:id="rId7" xr:uid="{EF37296B-2C4F-443E-8A62-5EBC2C7C912D}"/>
+    <hyperlink ref="H25" r:id="rId8" xr:uid="{D5CCAD84-AA32-46C6-8982-ED0BE724ED24}"/>
+    <hyperlink ref="H13" r:id="rId9" xr:uid="{1C4D161B-5B9A-48D8-8915-791C7D0D57F6}"/>
+    <hyperlink ref="H28" r:id="rId10" xr:uid="{A3E534BB-E017-4FD6-8571-6B29D0EC1106}"/>
+    <hyperlink ref="H9" r:id="rId11" xr:uid="{3A11E16B-FDBC-4C11-A8B9-5D70D3AF6CE1}"/>
+    <hyperlink ref="H8" r:id="rId12" xr:uid="{D967CC38-902E-4CFB-B295-BD12ED14CF46}"/>
+    <hyperlink ref="H21" r:id="rId13" xr:uid="{AA4253AA-A5F9-4D33-9C0C-D0D54386A28A}"/>
+    <hyperlink ref="H19" r:id="rId14" xr:uid="{E0CE1F9E-1805-40CE-ABC5-B9DD1FCAF543}"/>
+    <hyperlink ref="H22" r:id="rId15" xr:uid="{C8DA5180-F0CB-402F-8319-619DD97F760F}"/>
+    <hyperlink ref="H20" r:id="rId16" xr:uid="{FB4130F6-3C25-45EC-AA00-61634945DC3F}"/>
+    <hyperlink ref="H4" r:id="rId17" xr:uid="{EEA2A48A-87FD-4482-91B9-1FF201ECBDFE}"/>
+    <hyperlink ref="H5" r:id="rId18" xr:uid="{E1474B6E-8B4D-40B5-AB1E-FA6B4DD997D8}"/>
+    <hyperlink ref="H6" r:id="rId19" xr:uid="{BF7882F2-1EF5-456D-AC58-8DC01C06893D}"/>
+    <hyperlink ref="H7" r:id="rId20" xr:uid="{478BB94C-435A-440D-9965-610D80EE4528}"/>
+    <hyperlink ref="H14" r:id="rId21" xr:uid="{9F355800-7535-4B88-B262-C64C59E477C1}"/>
+    <hyperlink ref="H16" r:id="rId22" xr:uid="{DC75FD14-51FF-4299-9C9A-7D20A6F25D29}"/>
+    <hyperlink ref="H17" r:id="rId23" xr:uid="{5231848B-A283-4A46-840C-2C91C3616795}"/>
+    <hyperlink ref="H23" r:id="rId24" xr:uid="{017F9B11-4368-4CA1-A199-7BA86CC8FE01}"/>
+    <hyperlink ref="H26" r:id="rId25" xr:uid="{B5B7B496-3341-43BE-85CE-3C243D1EB096}"/>
+    <hyperlink ref="H27" r:id="rId26" xr:uid="{1C7CDA99-49DC-41E9-AA06-FEE25BA3567E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>